<commit_message>
version 1.0.0 is complete
</commit_message>
<xml_diff>
--- a/Geo Team/bin/Debug/data/Student Sheet 2022.xlsx
+++ b/Geo Team/bin/Debug/data/Student Sheet 2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abdelrahman\source\repos\Geo Team\Geo Team\bin\Debug\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27652B6D-1593-4ACA-A43B-F94036C6B4E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347BB0FB-E483-4A11-81FF-A28BEE6DC273}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
   <si>
     <t>code</t>
   </si>
@@ -106,6 +106,21 @@
   </si>
   <si>
     <t>16/05</t>
+  </si>
+  <si>
+    <t>alaa</t>
+  </si>
+  <si>
+    <t>01001002345</t>
+  </si>
+  <si>
+    <t>sayed</t>
+  </si>
+  <si>
+    <t>sat</t>
+  </si>
+  <si>
+    <t>yasmin</t>
   </si>
 </sst>
 </file>
@@ -472,10 +487,18 @@
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="A4" s="1">
+        <v>125</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -484,12 +507,24 @@
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="A5" s="1">
+        <v>126</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -3886,8 +3921,12 @@
       <c r="C1" s="2">
         <v>124</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="D1" s="3">
+        <v>125</v>
+      </c>
+      <c r="E1" s="3">
+        <v>126</v>
+      </c>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
@@ -4034,9 +4073,15 @@
       <c r="J9" s="3"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="A10" s="7">
+        <v>44290</v>
+      </c>
+      <c r="B10" s="3">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3">
+        <v>9</v>
+      </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>

</xml_diff>